<commit_message>
just update some png
</commit_message>
<xml_diff>
--- a/DataFileSamples/Stereographic and Rose map/Structure.xlsx
+++ b/DataFileSamples/Stereographic and Rose map/Structure.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/GeoCode/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/Stereographic and Rose map/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F243028C-C01B-154A-AB1C-0A4D39ECF018}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40600" yWindow="1940" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="10240" yWindow="1940" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -165,9 +166,6 @@
     <t>Group2</t>
   </si>
   <si>
-    <t>Group3</t>
-  </si>
-  <si>
     <t>Dip-Angle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -407,17 +405,20 @@
   </si>
   <si>
     <t>blue</t>
+  </si>
+  <si>
+    <t>Group1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,13 +461,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color theme="0"/>
-      <name val="仿宋"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -491,11 +485,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -513,23 +506,19 @@
     <xf numFmtId="177" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规_REE配分模式" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -797,16 +786,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="18">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -817,31 +806,31 @@
         <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="18">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -859,7 +848,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2">
         <v>50</v>
@@ -877,7 +866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="18">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -895,7 +884,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="2">
         <v>50</v>
@@ -913,7 +902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="18">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -931,7 +920,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="2">
         <v>50</v>
@@ -949,7 +938,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="18">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -967,7 +956,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" s="2">
         <v>50</v>
@@ -985,7 +974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="18">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +992,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="2">
         <v>50</v>
@@ -1021,7 +1010,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="18">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +1028,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="2">
         <v>50</v>
@@ -1057,7 +1046,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="18">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1064,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -1093,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="18">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1111,7 +1100,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G9" s="2">
         <v>50</v>
@@ -1129,7 +1118,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="18">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1136,7 @@
         <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" s="2">
         <v>50</v>
@@ -1165,7 +1154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="18">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1183,7 +1172,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G11" s="2">
         <v>50</v>
@@ -1201,7 +1190,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="18">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1219,7 +1208,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G12" s="2">
         <v>50</v>
@@ -1237,7 +1226,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="18">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1255,7 +1244,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" s="2">
         <v>50</v>
@@ -1273,7 +1262,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="18">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1291,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G14" s="2">
         <v>50</v>
@@ -1309,7 +1298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="18">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1327,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="2">
         <v>50</v>
@@ -1345,7 +1334,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="18">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1352,7 @@
         <v>31</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="2">
         <v>50</v>
@@ -1381,7 +1370,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="18">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1399,7 +1388,7 @@
         <v>31</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G17" s="2">
         <v>50</v>
@@ -1417,7 +1406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="18">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1435,7 +1424,7 @@
         <v>31</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -1453,7 +1442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="18">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1471,7 +1460,7 @@
         <v>31</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="2">
         <v>50</v>
@@ -1489,7 +1478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="18">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1507,7 +1496,7 @@
         <v>31</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G20" s="2">
         <v>50</v>
@@ -1525,7 +1514,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="18">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1543,7 +1532,7 @@
         <v>31</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2">
         <v>50</v>
@@ -1561,7 +1550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="18">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +1568,7 @@
         <v>31</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G22" s="2">
         <v>50</v>
@@ -1597,7 +1586,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="18">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1615,7 +1604,7 @@
         <v>31</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2">
         <v>50</v>
@@ -1633,7 +1622,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="18">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1651,7 +1640,7 @@
         <v>31</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G24" s="2">
         <v>50</v>
@@ -1669,7 +1658,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="18">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1687,7 +1676,7 @@
         <v>31</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G25" s="2">
         <v>50</v>
@@ -1705,9 +1694,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="18">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4">
         <v>34</v>
@@ -1723,7 +1712,7 @@
         <v>31</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G26" s="2">
         <v>50</v>
@@ -1741,9 +1730,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="18">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="4">
         <v>34</v>
@@ -1759,7 +1748,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G27" s="2">
         <v>50</v>
@@ -1777,9 +1766,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="18">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4">
         <v>34</v>
@@ -1795,7 +1784,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="2">
         <v>50</v>
@@ -1813,9 +1802,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="18">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="4">
         <v>35</v>
@@ -1831,7 +1820,7 @@
         <v>31</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G29" s="2">
         <v>50</v>
@@ -1849,9 +1838,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="18">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4">
         <v>36</v>
@@ -1867,7 +1856,7 @@
         <v>31</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G30" s="2">
         <v>50</v>
@@ -1885,9 +1874,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="18">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4">
         <v>34</v>
@@ -1903,7 +1892,7 @@
         <v>31</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G31" s="2">
         <v>50</v>
@@ -1921,9 +1910,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="18">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="4">
         <v>34</v>
@@ -1939,7 +1928,7 @@
         <v>31</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G32" s="2">
         <v>50</v>
@@ -1957,9 +1946,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="18">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="4">
         <v>35</v>
@@ -1975,7 +1964,7 @@
         <v>31</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G33" s="2">
         <v>50</v>
@@ -1993,9 +1982,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="18">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="4">
         <v>35</v>
@@ -2011,7 +2000,7 @@
         <v>31</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G34" s="2">
         <v>50</v>
@@ -2029,9 +2018,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="18">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" s="4">
         <v>35</v>
@@ -2047,7 +2036,7 @@
         <v>31</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G35" s="2">
         <v>50</v>
@@ -2065,9 +2054,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="18">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="4">
         <v>36</v>
@@ -2083,7 +2072,7 @@
         <v>31</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G36" s="2">
         <v>50</v>
@@ -2101,9 +2090,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="18">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="4">
         <v>36</v>
@@ -2119,7 +2108,7 @@
         <v>31</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G37" s="2">
         <v>50</v>
@@ -2137,9 +2126,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="18">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="4">
         <v>44</v>
@@ -2155,7 +2144,7 @@
         <v>31</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G38" s="2">
         <v>50</v>
@@ -2173,9 +2162,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="18">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="4">
         <v>44</v>
@@ -2191,7 +2180,7 @@
         <v>31</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G39" s="2">
         <v>50</v>
@@ -2209,9 +2198,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="18">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="4">
         <v>45</v>
@@ -2227,7 +2216,7 @@
         <v>31</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G40" s="2">
         <v>50</v>
@@ -2245,9 +2234,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="18">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="4">
         <v>45</v>
@@ -2263,7 +2252,7 @@
         <v>31</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G41" s="2">
         <v>50</v>
@@ -2281,9 +2270,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="18">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" s="4">
         <v>46</v>
@@ -2299,7 +2288,7 @@
         <v>31</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G42" s="2">
         <v>50</v>
@@ -2317,9 +2306,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="18">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="4">
         <v>46</v>
@@ -2335,7 +2324,7 @@
         <v>31</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G43" s="2">
         <v>50</v>
@@ -2353,9 +2342,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="18">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="4">
         <v>46</v>
@@ -2371,7 +2360,7 @@
         <v>31</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G44" s="2">
         <v>50</v>
@@ -2389,9 +2378,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="18">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="4">
         <v>46</v>
@@ -2407,7 +2396,7 @@
         <v>31</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G45" s="2">
         <v>50</v>
@@ -2425,9 +2414,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="18">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="4">
         <v>46</v>
@@ -2443,7 +2432,7 @@
         <v>31</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G46" s="2">
         <v>50</v>
@@ -2461,9 +2450,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="18">
       <c r="A47" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="4">
         <v>46</v>
@@ -2479,7 +2468,7 @@
         <v>31</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G47" s="2">
         <v>50</v>
@@ -2497,9 +2486,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="18">
       <c r="A48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="4">
         <v>46</v>
@@ -2515,7 +2504,7 @@
         <v>31</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G48" s="2">
         <v>50</v>
@@ -2533,9 +2522,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="18">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" s="4">
         <v>46</v>
@@ -2551,7 +2540,7 @@
         <v>31</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G49" s="2">
         <v>50</v>
@@ -2569,9 +2558,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="18">
       <c r="A50" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" s="4">
         <v>47</v>
@@ -2587,7 +2576,7 @@
         <v>31</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G50" s="2">
         <v>50</v>
@@ -2605,9 +2594,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="18">
       <c r="A51" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="4">
         <v>47</v>
@@ -2623,7 +2612,7 @@
         <v>31</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G51" s="2">
         <v>50</v>
@@ -2641,9 +2630,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="18">
       <c r="A52" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" s="4">
         <v>47</v>
@@ -2659,7 +2648,7 @@
         <v>31</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G52" s="2">
         <v>50</v>
@@ -2677,9 +2666,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="18">
       <c r="A53" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" s="4">
         <v>48</v>
@@ -2695,7 +2684,7 @@
         <v>31</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G53" s="2">
         <v>50</v>
@@ -2713,9 +2702,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="18">
       <c r="A54" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="4">
         <v>47</v>
@@ -2731,7 +2720,7 @@
         <v>31</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G54" s="2">
         <v>50</v>
@@ -2749,9 +2738,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="18">
       <c r="A55" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="4">
         <v>45</v>
@@ -2767,7 +2756,7 @@
         <v>31</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G55" s="2">
         <v>50</v>
@@ -2785,9 +2774,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="18">
       <c r="A56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="4">
         <v>45</v>
@@ -2803,7 +2792,7 @@
         <v>31</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G56" s="2">
         <v>50</v>
@@ -2821,9 +2810,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="18">
       <c r="A57" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" s="4">
         <v>46</v>
@@ -2839,7 +2828,7 @@
         <v>31</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G57" s="2">
         <v>50</v>
@@ -2857,9 +2846,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="18">
       <c r="A58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58" s="4">
         <v>46</v>
@@ -2875,7 +2864,7 @@
         <v>31</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G58" s="2">
         <v>50</v>
@@ -2893,9 +2882,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="18">
       <c r="A59" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59" s="4">
         <v>281</v>
@@ -2926,12 +2915,12 @@
         <v>0.5</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="18">
       <c r="A60" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60" s="4">
         <v>282</v>
@@ -2962,12 +2951,12 @@
         <v>0.5</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="18">
       <c r="A61" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61" s="4">
         <v>285</v>
@@ -2998,12 +2987,12 @@
         <v>0.5</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="18">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62" s="4">
         <v>292</v>
@@ -3034,12 +3023,12 @@
         <v>0.5</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="18">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="4">
         <v>293</v>
@@ -3070,12 +3059,12 @@
         <v>0.5</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="18">
       <c r="A64" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="4">
         <v>294</v>
@@ -3106,12 +3095,12 @@
         <v>0.5</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="18">
       <c r="A65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="4">
         <v>295</v>
@@ -3142,12 +3131,12 @@
         <v>0.5</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="18">
       <c r="A66" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="4">
         <v>294</v>
@@ -3178,12 +3167,12 @@
         <v>0.5</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="18">
       <c r="A67" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B67" s="4">
         <v>296</v>
@@ -3214,12 +3203,12 @@
         <v>0.5</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="18">
       <c r="A68" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="4">
         <v>306</v>
@@ -3250,12 +3239,12 @@
         <v>0.5</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="18">
       <c r="A69" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B69" s="4">
         <v>307</v>
@@ -3286,12 +3275,12 @@
         <v>0.5</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="18">
       <c r="A70" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B70" s="4">
         <v>305</v>
@@ -3322,12 +3311,12 @@
         <v>0.5</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="18">
       <c r="A71" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B71" s="4">
         <v>304</v>
@@ -3358,12 +3347,12 @@
         <v>0.5</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="18">
       <c r="A72" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B72" s="4">
         <v>305</v>
@@ -3394,12 +3383,12 @@
         <v>0.5</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="18">
       <c r="A73" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B73" s="4">
         <v>306</v>
@@ -3430,12 +3419,12 @@
         <v>0.5</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="18">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" s="4">
         <v>301</v>
@@ -3466,12 +3455,12 @@
         <v>0.5</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="18">
       <c r="A75" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B75" s="4">
         <v>302</v>
@@ -3502,12 +3491,12 @@
         <v>0.5</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="18">
       <c r="A76" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B76" s="4">
         <v>302</v>
@@ -3538,12 +3527,12 @@
         <v>0.5</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="18">
       <c r="A77" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B77" s="4">
         <v>304</v>
@@ -3574,12 +3563,12 @@
         <v>0.5</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="18">
       <c r="A78" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="4">
         <v>313</v>
@@ -3610,12 +3599,12 @@
         <v>0.5</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="18">
       <c r="A79" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" s="4">
         <v>313</v>
@@ -3646,12 +3635,12 @@
         <v>0.5</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="18">
       <c r="A80" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B80" s="4">
         <v>314</v>
@@ -3682,12 +3671,12 @@
         <v>0.5</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="18">
       <c r="A81" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B81" s="4">
         <v>315</v>
@@ -3718,12 +3707,12 @@
         <v>0.5</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="18">
       <c r="A82" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B82" s="4">
         <v>315</v>
@@ -3754,12 +3743,12 @@
         <v>0.5</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="18">
       <c r="A83" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B83" s="4">
         <v>315</v>
@@ -3790,12 +3779,12 @@
         <v>0.5</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="18">
       <c r="A84" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B84" s="4">
         <v>316</v>
@@ -3826,12 +3815,12 @@
         <v>0.5</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="18">
       <c r="A85" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B85" s="4">
         <v>319</v>
@@ -3862,12 +3851,12 @@
         <v>0.5</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="18">
       <c r="A86" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B86" s="4">
         <v>312</v>
@@ -3898,12 +3887,12 @@
         <v>0.5</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="18">
       <c r="A87" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B87" s="4">
         <v>314</v>
@@ -3934,12 +3923,12 @@
         <v>0.5</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="18">
       <c r="A88" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B88" s="4">
         <v>314</v>
@@ -3970,12 +3959,12 @@
         <v>0.5</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="18">
       <c r="A89" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B89" s="4">
         <v>314</v>
@@ -4006,12 +3995,12 @@
         <v>0.5</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="18">
       <c r="A90" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B90" s="4">
         <v>314</v>
@@ -4042,12 +4031,12 @@
         <v>0.5</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="18">
       <c r="A91" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B91" s="4">
         <v>316</v>
@@ -4078,12 +4067,12 @@
         <v>0.5</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="18">
       <c r="A92" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B92" s="4">
         <v>316</v>
@@ -4114,12 +4103,12 @@
         <v>0.5</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="18">
       <c r="A93" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B93" s="4">
         <v>317</v>
@@ -4150,12 +4139,12 @@
         <v>0.5</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="18">
       <c r="A94" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B94" s="4">
         <v>321</v>
@@ -4186,12 +4175,12 @@
         <v>0.5</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="18">
       <c r="A95" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B95" s="4">
         <v>324</v>
@@ -4222,12 +4211,12 @@
         <v>0.5</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="18">
       <c r="A96" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B96" s="4">
         <v>325</v>
@@ -4258,12 +4247,12 @@
         <v>0.5</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="18">
       <c r="A97" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B97" s="4">
         <v>325</v>
@@ -4294,12 +4283,12 @@
         <v>0.5</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="18">
       <c r="A98" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B98" s="4">
         <v>325</v>
@@ -4330,12 +4319,12 @@
         <v>0.5</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="18">
       <c r="A99" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B99" s="4">
         <v>325</v>
@@ -4366,12 +4355,12 @@
         <v>0.5</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="18">
       <c r="A100" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B100" s="4">
         <v>326</v>
@@ -4402,12 +4391,12 @@
         <v>0.5</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="18">
       <c r="A101" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B101" s="4">
         <v>329</v>
@@ -4438,12 +4427,12 @@
         <v>0.5</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="18">
       <c r="A102" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B102" s="4">
         <v>327</v>
@@ -4474,12 +4463,12 @@
         <v>0.5</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="18">
       <c r="A103" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" s="4">
         <v>329</v>
@@ -4510,7 +4499,7 @@
         <v>0.5</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>